<commit_message>
Final updates to REV B
</commit_message>
<xml_diff>
--- a/Fabrication/REV A/Interface Board BOM Rev A.xlsx
+++ b/Fabrication/REV A/Interface Board BOM Rev A.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Reid\Documents\KiCad Projects\Programmer Board\LMS-6_Interface_Board\Fabrication\REV A\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{03FDDFB4-3F55-4EB7-9FF6-B7DC7E92AF86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E426A681-89EC-4618-96C1-FD4C541FFE64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{16602299-295D-4FFD-99B9-8F34A34E12AC}"/>
   </bookViews>
@@ -725,7 +725,7 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>